<commit_message>
looked through code before starting dms work
</commit_message>
<xml_diff>
--- a/EA Waste Tonnage Returns/Documents/Config/config.xlsx
+++ b/EA Waste Tonnage Returns/Documents/Config/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dswindlehurst\Documents\Development\EA-Waste-Tonnage-Returns\EA Waste Tonnage Returns\Documents\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mewinter\Desktop\EA-Waste-Tonnage-Returns\EA Waste Tonnage Returns\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>timeoutS</t>
   </si>
@@ -132,6 +132,54 @@
   </si>
   <si>
     <t>boolProcessBreakout</t>
+  </si>
+  <si>
+    <t>DMSHomeUrl</t>
+  </si>
+  <si>
+    <t>DMSEmailTitle</t>
+  </si>
+  <si>
+    <t>DMSExcelReturnTitle</t>
+  </si>
+  <si>
+    <t>Compliance Waste Returns {1} {2}</t>
+  </si>
+  <si>
+    <t>Compliance Waste Returns {1} {2} - Email and Submission</t>
+  </si>
+  <si>
+    <t>DMSEmailDisclosureStatus</t>
+  </si>
+  <si>
+    <t>Internal Only</t>
+  </si>
+  <si>
+    <t>DMSExcelReturnDisclosureStatus</t>
+  </si>
+  <si>
+    <t>Public Register</t>
+  </si>
+  <si>
+    <t>Title to rename email file once uploaded to DMS</t>
+  </si>
+  <si>
+    <t>Title to rename excel return file once uploaded to DMS</t>
+  </si>
+  <si>
+    <t>Disclosure status for excel return file once uploaded to DMS</t>
+  </si>
+  <si>
+    <t>Disclosure status for email file once uploaded to DMS</t>
+  </si>
+  <si>
+    <t>Home url site for DMS</t>
+  </si>
+  <si>
+    <t>DMSPermitFolderUrl</t>
+  </si>
+  <si>
+    <t>Url for permit folder  on DMS</t>
   </si>
 </sst>
 </file>
@@ -257,8 +305,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C26" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C26"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Name" dataDxfId="2"/>
     <tableColumn id="2" name="Value" dataDxfId="1"/>
@@ -565,15 +613,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="69" style="4" customWidth="1"/>
     <col min="3" max="3" width="56" style="4" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="3"/>
@@ -774,13 +822,73 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
+    <row r="26" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added getting the subject from email for permit number, updating excel permit with new permit number, and added dms library
</commit_message>
<xml_diff>
--- a/EA Waste Tonnage Returns/Documents/Config/config.xlsx
+++ b/EA Waste Tonnage Returns/Documents/Config/config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>timeoutS</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>Url for permit folder  on DMS</t>
+  </si>
+  <si>
+    <t>https://defradev.sharepoint.com/sites/EADMSRoboticsHomeSite</t>
   </si>
 </sst>
 </file>
@@ -616,7 +619,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,6 +828,9 @@
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="B19" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
published new dms library, added workflow to remove DOB from excel return, and upload file to dms
</commit_message>
<xml_diff>
--- a/EA Waste Tonnage Returns/Documents/Config/config.xlsx
+++ b/EA Waste Tonnage Returns/Documents/Config/config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>timeoutS</t>
   </si>
@@ -146,9 +146,6 @@
     <t>Compliance Waste Returns {1} {2}</t>
   </si>
   <si>
-    <t>Compliance Waste Returns {1} {2} - Email and Submission</t>
-  </si>
-  <si>
     <t>DMSEmailDisclosureStatus</t>
   </si>
   <si>
@@ -176,13 +173,37 @@
     <t>Home url site for DMS</t>
   </si>
   <si>
-    <t>DMSPermitFolderUrl</t>
-  </si>
-  <si>
-    <t>Url for permit folder  on DMS</t>
-  </si>
-  <si>
     <t>https://defradev.sharepoint.com/sites/EADMSRoboticsHomeSite</t>
+  </si>
+  <si>
+    <t>https://defradev.sharepoint.com/sites/EADMSRobotics1/</t>
+  </si>
+  <si>
+    <t>DMSSiteUrl</t>
+  </si>
+  <si>
+    <t>Url for DMS site</t>
+  </si>
+  <si>
+    <t>DMSDocumentUrl</t>
+  </si>
+  <si>
+    <t>Url for where the document will be uploaded to</t>
+  </si>
+  <si>
+    <t>DMSReturnFolderUrl</t>
+  </si>
+  <si>
+    <t>Url for return folder on DMS</t>
+  </si>
+  <si>
+    <t>https://defradev.sharepoint.com/sites/EADMSRobotics1/LIB1/{0}/Returns</t>
+  </si>
+  <si>
+    <t>/sites/EADMSRobotics1/LIB1/{0}/Returns/{1}{2}</t>
+  </si>
+  <si>
+    <t>Compliance Waste Returns {0} {1} - Email and Submission</t>
   </si>
 </sst>
 </file>
@@ -236,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -258,6 +279,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -308,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C26" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C28" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C28"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Name" dataDxfId="2"/>
     <tableColumn id="2" name="Value" dataDxfId="1"/>
@@ -616,16 +643,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69" style="4" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="56" style="4" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
@@ -829,72 +856,97 @@
         <v>36</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>40</v>
+        <v>55</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
+    <row r="28" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes and additions to dms workflows
</commit_message>
<xml_diff>
--- a/EA Waste Tonnage Returns/Documents/Config/config.xlsx
+++ b/EA Waste Tonnage Returns/Documents/Config/config.xlsx
@@ -143,9 +143,6 @@
     <t>DMSExcelReturnTitle</t>
   </si>
   <si>
-    <t>Compliance Waste Returns {1} {2}</t>
-  </si>
-  <si>
     <t>DMSEmailDisclosureStatus</t>
   </si>
   <si>
@@ -203,7 +200,10 @@
     <t>/sites/EADMSRobotics1/LIB1/{0}/Returns/{1}{2}</t>
   </si>
   <si>
-    <t>Compliance Waste Returns {0} {1} - Email and Submission</t>
+    <t>Compliance Waste Returns{0} {1}</t>
+  </si>
+  <si>
+    <t>Compliance Waste Returns{0} {1} - Email and Submission</t>
   </si>
 </sst>
 </file>
@@ -646,7 +646,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,43 +856,43 @@
         <v>36</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -903,18 +903,18 @@
         <v>59</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="C24" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -922,21 +922,21 @@
         <v>38</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="C26" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding variables to upload excel return to dms to work with process case
</commit_message>
<xml_diff>
--- a/EA Waste Tonnage Returns/Documents/Config/config.xlsx
+++ b/EA Waste Tonnage Returns/Documents/Config/config.xlsx
@@ -200,10 +200,10 @@
     <t>/sites/EADMSRobotics1/LIB1/{0}/Returns/{1}{2}</t>
   </si>
   <si>
-    <t>Compliance Waste Returns{0} {1}</t>
-  </si>
-  <si>
-    <t>Compliance Waste Returns{0} {1} - Email and Submission</t>
+    <t>Compliance Waste Returns {0} {1}</t>
+  </si>
+  <si>
+    <t>Compliance Waste Returns {0} {1} - Email and Submission</t>
   </si>
 </sst>
 </file>
@@ -646,7 +646,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changes from deploying and adding live\test config
</commit_message>
<xml_diff>
--- a/EA Waste Tonnage Returns/Documents/Config/config.xlsx
+++ b/EA Waste Tonnage Returns/Documents/Config/config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>timeoutS</t>
   </si>
@@ -204,6 +204,15 @@
   </si>
   <si>
     <t>/sites/EADMSRobotics1/LIB1/{0}/Returns/{1}</t>
+  </si>
+  <si>
+    <t>EmailAccount</t>
+  </si>
+  <si>
+    <t>national-operator-returns@environment-agency.gov.uk</t>
+  </si>
+  <si>
+    <t>Email account used for the emails being processed by the robot</t>
   </si>
 </sst>
 </file>
@@ -335,8 +344,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C28" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C29" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C29"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Name" dataDxfId="2"/>
     <tableColumn id="2" name="Value" dataDxfId="1"/>
@@ -643,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,100 +862,111 @@
     </row>
     <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>49</v>
+        <v>36</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>56</v>
+        <v>50</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
+    <row r="29" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes to timeouts for uploading return to orats
</commit_message>
<xml_diff>
--- a/EA Waste Tonnage Returns/Documents/Config/config.xlsx
+++ b/EA Waste Tonnage Returns/Documents/Config/config.xlsx
@@ -654,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +821,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="4">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>25</v>

</xml_diff>